<commit_message>
Importar Datos Relacionados con validaciones
</commit_message>
<xml_diff>
--- a/public/DataUpload/users-FE-1.xlsx
+++ b/public/DataUpload/users-FE-1.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
   <si>
     <t xml:space="preserve">first_name</t>
   </si>
@@ -56,12 +56,6 @@
   </si>
   <si>
     <t xml:space="preserve">heaney.rodolfo@example.net</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Prof. Edward Casper IV</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rene57@example.net</t>
   </si>
   <si>
     <t xml:space="preserve">Vella Moen</t>
@@ -179,13 +173,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="27.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="1" width="30.47"/>
@@ -270,7 +264,7 @@
       <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D6" s="1" t="s">
@@ -278,24 +272,10 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="C7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="2"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>